<commit_message>
updated Readme & fixed RCF -> RFC
</commit_message>
<xml_diff>
--- a/docs/excel/ResearchAndrequirements.xlsx
+++ b/docs/excel/ResearchAndrequirements.xlsx
@@ -5,15 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willg\Documents\Ubuntu-Webdev\packages-dev\DynamicCodeNinja\OAuth2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willg\Documents\Ubuntu-Webdev\packages-dev\DynamicCodeNinja\OAuth2\docs\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{238F23C5-3232-410B-A924-87093B0728AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC452CEE-1326-4987-AA90-91CD960912AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{5DED5BA5-C0FD-470C-B1A9-541329CA2D3E}"/>
   </bookViews>
   <sheets>
     <sheet name="RFCs" sheetId="1" r:id="rId1"/>
+    <sheet name="Definitions" sheetId="5" r:id="rId2"/>
+    <sheet name="Roles" sheetId="9" r:id="rId3"/>
+    <sheet name="Requirements" sheetId="10" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
   <si>
     <t>https://tools.ietf.org/html/rfc6749</t>
   </si>
@@ -167,7 +170,116 @@
     <t>OAuth 2.0 Device Authorization Grant</t>
   </si>
   <si>
-    <t>https://tools.ietf.org/wg/oauth/</t>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>SHALL</t>
+  </si>
+  <si>
+    <t>Client Developer</t>
+  </si>
+  <si>
+    <t>SHOULD NOT</t>
+  </si>
+  <si>
+    <t>SHOULD</t>
+  </si>
+  <si>
+    <t>MUST NOT</t>
+  </si>
+  <si>
+    <t>MAY</t>
+  </si>
+  <si>
+    <t>MUST</t>
+  </si>
+  <si>
+    <t>Section</t>
+  </si>
+  <si>
+    <t>NOT RECOMMENDED</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>This word, or the terms "REQUIRED" or "SHALL", mean that the definition is an absolute requirement of the specification.</t>
+  </si>
+  <si>
+    <t>This phrase, or the phrase "SHALL NOT", mean that the definition is an absolute prohibition of the specification.</t>
+  </si>
+  <si>
+    <t>This word, or the adjective "RECOMMENDED", mean that there may exist valid reasons in particular circumstances to ignore a particular item, but the full implications must be understood and carefully weighed before choosing a different course.</t>
+  </si>
+  <si>
+    <t>This phrase, or the phrase "NOT RECOMMENDED" mean that there may exist valid reasons in particular circumstances when the particular behavior is acceptable or even useful, but the full implications should be understood and the case carefully weighed before implementing any behavior described with this label.</t>
+  </si>
+  <si>
+    <t>This word, or the adjective "OPTIONAL", mean that an item is truly optional.  One vendor may choose to include the item because a particular marketplace requires it or because the vendor feels that it enhances the product while another vendor may omit the same item.
+An implementation which does not include a particular option MUST be prepared to interoperate with another implementation which does include the option, though perhaps with reduced functionality. In the same vein an implementation which does include a particular option MUST be prepared to interoperate with another implementation which does not include the option (except, of course, for the feature the option provides.)</t>
+  </si>
+  <si>
+    <t>REQUIRED</t>
+  </si>
+  <si>
+    <t>SHALL NOT</t>
+  </si>
+  <si>
+    <t>RECOMMENDED</t>
+  </si>
+  <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
+    <t>Resource Owner</t>
+  </si>
+  <si>
+    <t>An entity capable of granting access to a protected resource. When the resource owner is a person, it is referred to as an end-user.</t>
+  </si>
+  <si>
+    <t>Resource Server</t>
+  </si>
+  <si>
+    <t>The server hosting the protected resources, capable of accepting and responding to protected resource requests using access tokens</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>An application making protected resource requests on behalf of the resource owner and with its authorization.  The term "client" does not imply any particular implementation characteristics (e.g., whether the application executes on a server, a desktop, or other devices).</t>
+  </si>
+  <si>
+    <t>Authorization Server</t>
+  </si>
+  <si>
+    <t>The server issuing access tokens to the client after successfully authenticating the resource owner and obtaining authorization.</t>
+  </si>
+  <si>
+    <t>RCF</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Mandate</t>
+  </si>
+  <si>
+    <t>Brief Description</t>
+  </si>
+  <si>
+    <t>Explicit Description</t>
+  </si>
+  <si>
+    <t>Sub-Role</t>
+  </si>
+  <si>
+    <t>The party responsible for creating and maintaining the client</t>
   </si>
 </sst>
 </file>
@@ -212,14 +324,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -237,6 +346,57 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1F53BEA1-B41A-4F66-986B-7A3CF4F72F91}" name="Table3" displayName="Table3" ref="A1:D1048575" totalsRowShown="0">
+  <autoFilter ref="A1:D1048575" xr:uid="{5D544347-9DF2-4AFA-BD61-5978F8A859C9}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{020A2455-65D9-4E87-AB2A-DC1C49271943}" name="ID"/>
+    <tableColumn id="2" xr3:uid="{AD04FCAD-63AD-4790-9BE0-3C937505CF73}" name="Updates"/>
+    <tableColumn id="3" xr3:uid="{35E93955-2133-4F0B-AA98-9A2F4D80837E}" name="Link"/>
+    <tableColumn id="4" xr3:uid="{D1792036-0144-405A-AE7B-E25871BCCA9E}" name="Title"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{DE41F306-2033-4058-A1F4-0F3463906B4A}" name="Table5" displayName="Table5" ref="A1:B1048576" totalsRowShown="0">
+  <autoFilter ref="A1:B1048576" xr:uid="{FFE44EE8-AC80-4A53-86C2-9A46A7A58142}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{18F13A48-9372-48E5-ABC4-D49A85139BAB}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{0350A107-F0DE-4C46-92AB-8FFE48174796}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{C95D2321-FE51-4BA6-8D05-2A05322009AB}" name="Table7" displayName="Table7" ref="A1:B1048576" totalsRowShown="0">
+  <autoFilter ref="A1:B1048576" xr:uid="{A4B4402D-9863-4C5C-B119-3F7FF016A84F}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{C3A4EDCC-5292-4763-BB9E-44940C3686F2}" name="Name"/>
+    <tableColumn id="2" xr3:uid="{C3862B6A-6AA4-48FC-BC8B-2EC8D4D37905}" name="Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{D62C847D-4349-4C84-8094-94DE67FD53B9}" name="Table8" displayName="Table8" ref="A1:G1048576" totalsRowShown="0">
+  <autoFilter ref="A1:G1048576" xr:uid="{7ECAC244-027A-4EEA-A3FD-C5F4435CDDA9}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{F4E93FA4-3BA6-48EC-AA60-907772B23EDB}" name="RCF"/>
+    <tableColumn id="2" xr3:uid="{3BAAA288-A050-401C-B103-414588178EDA}" name="Section"/>
+    <tableColumn id="3" xr3:uid="{92644BFB-F554-4CA7-BF19-595F96EB3610}" name="Role"/>
+    <tableColumn id="7" xr3:uid="{9A1BCC20-80CF-42DF-9362-CD8B40108AD4}" name="Sub-Role"/>
+    <tableColumn id="4" xr3:uid="{66D8FF8E-FC71-4C48-92BD-D8355F47F00D}" name="Mandate"/>
+    <tableColumn id="5" xr3:uid="{9084E918-F055-42FB-86C5-5F4F3FEDD362}" name="Brief Description"/>
+    <tableColumn id="6" xr3:uid="{4E03BA7F-7F24-4DED-87BE-4440D0643F36}" name="Explicit Description"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,293 +696,535 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB555161-7E63-45FA-AC83-31A469F90E45}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
     <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="106.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
+      <c r="A2">
+        <v>6749</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
+        <v>8252</v>
+      </c>
+      <c r="B3">
         <v>6749</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="D3" t="s">
-        <v>1</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>8252</v>
-      </c>
-      <c r="B4">
-        <v>6749</v>
+        <v>7519</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
+        <v>7797</v>
+      </c>
+      <c r="B5">
         <v>7519</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>7797</v>
-      </c>
-      <c r="B6">
-        <v>7519</v>
+        <v>6750</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6750</v>
+        <v>6819</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6819</v>
+        <v>7662</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7662</v>
+        <v>7009</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>7009</v>
+        <v>8414</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>8414</v>
+        <v>7591</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>7591</v>
+        <v>7521</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>7521</v>
+        <v>7522</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>7522</v>
+        <v>7523</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>7523</v>
+        <v>6755</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D15" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>6755</v>
+        <v>8693</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>8693</v>
+        <v>7636</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>7636</v>
+        <v>7800</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>7800</v>
+        <v>7592</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7592</v>
+        <v>8176</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>8176</v>
+        <v>8628</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>8628</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D22" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{E7F146FA-5938-44DE-8B15-8E339C2E4F8B}"/>
-    <hyperlink ref="C7" r:id="rId2" xr:uid="{2659E989-BD34-4A6F-84F0-BDC99BFEBDDE}"/>
-    <hyperlink ref="C8" r:id="rId3" xr:uid="{383627A1-9A8A-4FDE-B9D8-3326EAB0ACED}"/>
-    <hyperlink ref="C9" r:id="rId4" xr:uid="{55237E76-0DF3-4937-8DDA-AA70DD9532A8}"/>
-    <hyperlink ref="C10" r:id="rId5" xr:uid="{9C6EDD42-23D0-4A20-8EE7-60C573433C5E}"/>
-    <hyperlink ref="C5" r:id="rId6" xr:uid="{FDB6281D-7FE3-434C-8141-FE8C4608AA95}"/>
-    <hyperlink ref="C11" r:id="rId7" xr:uid="{30B73139-7E44-4741-BD88-D568A7FCC3FE}"/>
-    <hyperlink ref="C12" r:id="rId8" xr:uid="{5BDE5620-09C8-45F5-B610-D1E5D1B7FDCB}"/>
-    <hyperlink ref="C13" r:id="rId9" xr:uid="{26C783B1-14CB-4B36-92F5-F8061E0EAEF1}"/>
-    <hyperlink ref="C14" r:id="rId10" xr:uid="{F465EB53-0515-4E02-8730-A2AB99B2E79D}"/>
-    <hyperlink ref="C15" r:id="rId11" xr:uid="{287FD97F-CCAB-4794-A280-BB74D15691C7}"/>
-    <hyperlink ref="C4" r:id="rId12" xr:uid="{E54F8251-C24B-4B1E-B7DB-F8760994FA53}"/>
-    <hyperlink ref="C6" r:id="rId13" xr:uid="{DBA365FA-E6C8-46B0-9D3D-7EE08083A588}"/>
-    <hyperlink ref="C16" r:id="rId14" xr:uid="{730CF362-626D-41D6-BE3F-DA039C5E56F9}"/>
-    <hyperlink ref="C17" r:id="rId15" xr:uid="{A15DFEF9-EC2D-4E18-B94F-38BFE2A93E2B}"/>
-    <hyperlink ref="C18" r:id="rId16" xr:uid="{24F440CB-6B42-408A-8208-01147605D9F4}"/>
-    <hyperlink ref="C19" r:id="rId17" xr:uid="{59918CC0-2053-482C-9027-A90E4D0F7A9B}"/>
-    <hyperlink ref="C20" r:id="rId18" xr:uid="{FC0B5ACB-433D-4E78-89CC-AF866CDBD34E}"/>
-    <hyperlink ref="C21" r:id="rId19" xr:uid="{847E4E8E-A051-4A8F-A151-81B1B997DA78}"/>
-    <hyperlink ref="C22" r:id="rId20" xr:uid="{86389E9C-E5C0-4340-BD8F-F8A726295702}"/>
-    <hyperlink ref="A1" r:id="rId21" xr:uid="{06559AF6-69A2-4159-930D-B7B939C8D30C}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{E7F146FA-5938-44DE-8B15-8E339C2E4F8B}"/>
+    <hyperlink ref="C6" r:id="rId2" xr:uid="{2659E989-BD34-4A6F-84F0-BDC99BFEBDDE}"/>
+    <hyperlink ref="C7" r:id="rId3" xr:uid="{383627A1-9A8A-4FDE-B9D8-3326EAB0ACED}"/>
+    <hyperlink ref="C8" r:id="rId4" xr:uid="{55237E76-0DF3-4937-8DDA-AA70DD9532A8}"/>
+    <hyperlink ref="C9" r:id="rId5" xr:uid="{9C6EDD42-23D0-4A20-8EE7-60C573433C5E}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{FDB6281D-7FE3-434C-8141-FE8C4608AA95}"/>
+    <hyperlink ref="C10" r:id="rId7" xr:uid="{30B73139-7E44-4741-BD88-D568A7FCC3FE}"/>
+    <hyperlink ref="C11" r:id="rId8" xr:uid="{5BDE5620-09C8-45F5-B610-D1E5D1B7FDCB}"/>
+    <hyperlink ref="C12" r:id="rId9" xr:uid="{26C783B1-14CB-4B36-92F5-F8061E0EAEF1}"/>
+    <hyperlink ref="C13" r:id="rId10" xr:uid="{F465EB53-0515-4E02-8730-A2AB99B2E79D}"/>
+    <hyperlink ref="C14" r:id="rId11" xr:uid="{287FD97F-CCAB-4794-A280-BB74D15691C7}"/>
+    <hyperlink ref="C3" r:id="rId12" xr:uid="{E54F8251-C24B-4B1E-B7DB-F8760994FA53}"/>
+    <hyperlink ref="C5" r:id="rId13" xr:uid="{DBA365FA-E6C8-46B0-9D3D-7EE08083A588}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{730CF362-626D-41D6-BE3F-DA039C5E56F9}"/>
+    <hyperlink ref="C16" r:id="rId15" xr:uid="{A15DFEF9-EC2D-4E18-B94F-38BFE2A93E2B}"/>
+    <hyperlink ref="C17" r:id="rId16" xr:uid="{24F440CB-6B42-408A-8208-01147605D9F4}"/>
+    <hyperlink ref="C18" r:id="rId17" xr:uid="{59918CC0-2053-482C-9027-A90E4D0F7A9B}"/>
+    <hyperlink ref="C19" r:id="rId18" xr:uid="{FC0B5ACB-433D-4E78-89CC-AF866CDBD34E}"/>
+    <hyperlink ref="C20" r:id="rId19" xr:uid="{847E4E8E-A051-4A8F-A151-81B1B997DA78}"/>
+    <hyperlink ref="C21" r:id="rId20" xr:uid="{86389E9C-E5C0-4340-BD8F-F8A726295702}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId21"/>
+  <tableParts count="1">
+    <tablePart r:id="rId22"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA6F2784-8F95-4A09-A91E-128F8738B744}">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>50</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E512FF98-2101-485C-A449-4EB2C25A985F}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="119.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B5" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEBBF160-307A-4CB3-BF9C-04C94A5F093B}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>6749</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="3">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F09BB29D-062E-48BA-8D3A-3254F96FC7CD}">
+          <x14:formula1>
+            <xm:f>RFCs!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>A1:A1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F93CE1CC-703B-41F9-BE1A-0C07C9D422C0}">
+          <x14:formula1>
+            <xm:f>Roles!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>C1:C1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{115A4393-8EC4-482B-8D5C-FCE793D2C0AE}">
+          <x14:formula1>
+            <xm:f>Definitions!$A:$A</xm:f>
+          </x14:formula1>
+          <xm:sqref>E1:E1048576</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>